<commit_message>
Update code for report co so
</commit_message>
<xml_diff>
--- a/notion_data/CHAM_CONG_CAN_THO.xlsx
+++ b/notion_data/CHAM_CONG_CAN_THO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EI14"/>
+  <dimension ref="A1:EL14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1101,30 +1101,45 @@
       </c>
       <c r="ED1" s="1" t="inlineStr">
         <is>
+          <t>properties.Ngày 7.select.id</t>
+        </is>
+      </c>
+      <c r="EE1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 7.select.name</t>
+        </is>
+      </c>
+      <c r="EF1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 7.select.color</t>
+        </is>
+      </c>
+      <c r="EG1" s="1" t="inlineStr">
+        <is>
           <t>properties.Ngày 1.select.id</t>
         </is>
       </c>
-      <c r="EE1" s="1" t="inlineStr">
+      <c r="EH1" s="1" t="inlineStr">
         <is>
           <t>properties.Ngày 1.select.name</t>
         </is>
       </c>
-      <c r="EF1" s="1" t="inlineStr">
+      <c r="EI1" s="1" t="inlineStr">
         <is>
           <t>properties.Ngày 1.select.color</t>
         </is>
       </c>
-      <c r="EG1" s="1" t="inlineStr">
+      <c r="EJ1" s="1" t="inlineStr">
         <is>
           <t>properties.Ngày 4.select.id</t>
         </is>
       </c>
-      <c r="EH1" s="1" t="inlineStr">
+      <c r="EK1" s="1" t="inlineStr">
         <is>
           <t>properties.Ngày 4.select.name</t>
         </is>
       </c>
-      <c r="EI1" s="1" t="inlineStr">
+      <c r="EL1" s="1" t="inlineStr">
         <is>
           <t>properties.Ngày 4.select.color</t>
         </is>
@@ -1612,6 +1627,9 @@
       <c r="EG2" t="inlineStr"/>
       <c r="EH2" t="inlineStr"/>
       <c r="EI2" t="inlineStr"/>
+      <c r="EJ2" t="inlineStr"/>
+      <c r="EK2" t="inlineStr"/>
+      <c r="EL2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2095,6 +2113,9 @@
       <c r="EG3" t="inlineStr"/>
       <c r="EH3" t="inlineStr"/>
       <c r="EI3" t="inlineStr"/>
+      <c r="EJ3" t="inlineStr"/>
+      <c r="EK3" t="inlineStr"/>
+      <c r="EL3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2578,6 +2599,9 @@
       <c r="EG4" t="inlineStr"/>
       <c r="EH4" t="inlineStr"/>
       <c r="EI4" t="inlineStr"/>
+      <c r="EJ4" t="inlineStr"/>
+      <c r="EK4" t="inlineStr"/>
+      <c r="EL4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3061,6 +3085,9 @@
       <c r="EG5" t="inlineStr"/>
       <c r="EH5" t="inlineStr"/>
       <c r="EI5" t="inlineStr"/>
+      <c r="EJ5" t="inlineStr"/>
+      <c r="EK5" t="inlineStr"/>
+      <c r="EL5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -3080,7 +3107,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-06T09:52:00.000Z</t>
+          <t>2024-07-07T12:43:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -3588,30 +3615,45 @@
       </c>
       <c r="ED6" t="inlineStr">
         <is>
+          <t>VRLp</t>
+        </is>
+      </c>
+      <c r="EE6" t="inlineStr">
+        <is>
+          <t>Nghỉ có phép</t>
+        </is>
+      </c>
+      <c r="EF6" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="EG6" t="inlineStr">
+        <is>
           <t>DjwF</t>
         </is>
       </c>
-      <c r="EE6" t="inlineStr">
+      <c r="EH6" t="inlineStr">
         <is>
           <t>Đầy đủ</t>
         </is>
       </c>
-      <c r="EF6" t="inlineStr">
+      <c r="EI6" t="inlineStr">
         <is>
           <t>pink</t>
         </is>
       </c>
-      <c r="EG6" t="inlineStr">
+      <c r="EJ6" t="inlineStr">
         <is>
           <t>DjwF</t>
         </is>
       </c>
-      <c r="EH6" t="inlineStr">
+      <c r="EK6" t="inlineStr">
         <is>
           <t>Đầy đủ</t>
         </is>
       </c>
-      <c r="EI6" t="inlineStr">
+      <c r="EL6" t="inlineStr">
         <is>
           <t>pink</t>
         </is>
@@ -3635,7 +3677,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-06T09:52:00.000Z</t>
+          <t>2024-07-07T12:43:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -4143,30 +4185,45 @@
       </c>
       <c r="ED7" t="inlineStr">
         <is>
+          <t>DjwF</t>
+        </is>
+      </c>
+      <c r="EE7" t="inlineStr">
+        <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EF7" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EG7" t="inlineStr">
+        <is>
           <t>VRLp</t>
         </is>
       </c>
-      <c r="EE7" t="inlineStr">
+      <c r="EH7" t="inlineStr">
         <is>
           <t>Nghỉ có phép</t>
         </is>
       </c>
-      <c r="EF7" t="inlineStr">
+      <c r="EI7" t="inlineStr">
         <is>
           <t>blue</t>
         </is>
       </c>
-      <c r="EG7" t="inlineStr">
+      <c r="EJ7" t="inlineStr">
         <is>
           <t>DjwF</t>
         </is>
       </c>
-      <c r="EH7" t="inlineStr">
+      <c r="EK7" t="inlineStr">
         <is>
           <t>Đầy đủ</t>
         </is>
       </c>
-      <c r="EI7" t="inlineStr">
+      <c r="EL7" t="inlineStr">
         <is>
           <t>pink</t>
         </is>
@@ -4654,6 +4711,9 @@
       <c r="EG8" t="inlineStr"/>
       <c r="EH8" t="inlineStr"/>
       <c r="EI8" t="inlineStr"/>
+      <c r="EJ8" t="inlineStr"/>
+      <c r="EK8" t="inlineStr"/>
+      <c r="EL8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -4673,7 +4733,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-06T09:52:00.000Z</t>
+          <t>2024-07-07T12:43:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -5209,6 +5269,21 @@
           <t>pink</t>
         </is>
       </c>
+      <c r="EJ9" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
+      <c r="EK9" t="inlineStr">
+        <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL9" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -5228,7 +5303,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-06T09:52:00.000Z</t>
+          <t>2024-07-07T12:43:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -5760,6 +5835,21 @@
         </is>
       </c>
       <c r="EI10" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EJ10" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
+      <c r="EK10" t="inlineStr">
+        <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL10" t="inlineStr">
         <is>
           <t>pink</t>
         </is>
@@ -6247,6 +6337,9 @@
       <c r="EG11" t="inlineStr"/>
       <c r="EH11" t="inlineStr"/>
       <c r="EI11" t="inlineStr"/>
+      <c r="EJ11" t="inlineStr"/>
+      <c r="EK11" t="inlineStr"/>
+      <c r="EL11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -6730,6 +6823,9 @@
       <c r="EG12" t="inlineStr"/>
       <c r="EH12" t="inlineStr"/>
       <c r="EI12" t="inlineStr"/>
+      <c r="EJ12" t="inlineStr"/>
+      <c r="EK12" t="inlineStr"/>
+      <c r="EL12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -7213,6 +7309,9 @@
       <c r="EG13" t="inlineStr"/>
       <c r="EH13" t="inlineStr"/>
       <c r="EI13" t="inlineStr"/>
+      <c r="EJ13" t="inlineStr"/>
+      <c r="EK13" t="inlineStr"/>
+      <c r="EL13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -7232,7 +7331,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-06T09:51:00.000Z</t>
+          <t>2024-07-07T12:42:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -7764,6 +7863,21 @@
         </is>
       </c>
       <c r="EI14" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EJ14" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
+      <c r="EK14" t="inlineStr">
+        <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL14" t="inlineStr">
         <is>
           <t>pink</t>
         </is>

</xml_diff>

<commit_message>
Update code for caclular Luong ca nhan
</commit_message>
<xml_diff>
--- a/notion_data/CHAM_CONG_CAN_THO.xlsx
+++ b/notion_data/CHAM_CONG_CAN_THO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FM20"/>
+  <dimension ref="A1:FP20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1081,200 +1081,215 @@
       </c>
       <c r="DZ1" s="1" t="inlineStr">
         <is>
+          <t>properties.Ngày 17.select.id</t>
+        </is>
+      </c>
+      <c r="EA1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 17.select.name</t>
+        </is>
+      </c>
+      <c r="EB1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 17.select.color</t>
+        </is>
+      </c>
+      <c r="EC1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 8.id</t>
+        </is>
+      </c>
+      <c r="ED1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 8.type</t>
+        </is>
+      </c>
+      <c r="EE1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 8.select.id</t>
+        </is>
+      </c>
+      <c r="EF1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 8.select.name</t>
+        </is>
+      </c>
+      <c r="EG1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 8.select.color</t>
+        </is>
+      </c>
+      <c r="EH1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 4.id</t>
+        </is>
+      </c>
+      <c r="EI1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 4.type</t>
+        </is>
+      </c>
+      <c r="EJ1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 4.select.id</t>
+        </is>
+      </c>
+      <c r="EK1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 4.select.name</t>
+        </is>
+      </c>
+      <c r="EL1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 4.select.color</t>
+        </is>
+      </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Cơ sở.id</t>
+        </is>
+      </c>
+      <c r="EN1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Cơ sở.type</t>
+        </is>
+      </c>
+      <c r="EO1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Cơ sở.rollup.type</t>
+        </is>
+      </c>
+      <c r="EP1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Cơ sở.rollup.array</t>
+        </is>
+      </c>
+      <c r="EQ1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Cơ sở.rollup.function</t>
+        </is>
+      </c>
+      <c r="ER1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 14.id</t>
+        </is>
+      </c>
+      <c r="ES1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 14.type</t>
+        </is>
+      </c>
+      <c r="ET1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 14.select.id</t>
+        </is>
+      </c>
+      <c r="EU1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 14.select.name</t>
+        </is>
+      </c>
+      <c r="EV1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 14.select.color</t>
+        </is>
+      </c>
+      <c r="EW1" s="1" t="inlineStr">
+        <is>
+          <t>properties.STT.id</t>
+        </is>
+      </c>
+      <c r="EX1" s="1" t="inlineStr">
+        <is>
+          <t>properties.STT.type</t>
+        </is>
+      </c>
+      <c r="EY1" s="1" t="inlineStr">
+        <is>
+          <t>properties.STT.title</t>
+        </is>
+      </c>
+      <c r="EZ1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 6.select</t>
+        </is>
+      </c>
+      <c r="FA1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 5.select</t>
+        </is>
+      </c>
+      <c r="FB1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 11.select</t>
+        </is>
+      </c>
+      <c r="FC1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 3.select</t>
+        </is>
+      </c>
+      <c r="FD1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 12.select</t>
+        </is>
+      </c>
+      <c r="FE1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 10.select</t>
+        </is>
+      </c>
+      <c r="FF1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 2.select</t>
+        </is>
+      </c>
+      <c r="FG1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 7.select</t>
+        </is>
+      </c>
+      <c r="FH1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 1.select</t>
+        </is>
+      </c>
+      <c r="FI1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 9.select</t>
+        </is>
+      </c>
+      <c r="FJ1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 16.select</t>
+        </is>
+      </c>
+      <c r="FK1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 15.select</t>
+        </is>
+      </c>
+      <c r="FL1" s="1" t="inlineStr">
+        <is>
+          <t>properties.Ngày 13.select</t>
+        </is>
+      </c>
+      <c r="FM1" s="1" t="inlineStr">
+        <is>
           <t>properties.Ngày 17.select</t>
         </is>
       </c>
-      <c r="EA1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 8.id</t>
-        </is>
-      </c>
-      <c r="EB1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 8.type</t>
-        </is>
-      </c>
-      <c r="EC1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 8.select.id</t>
-        </is>
-      </c>
-      <c r="ED1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 8.select.name</t>
-        </is>
-      </c>
-      <c r="EE1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 8.select.color</t>
-        </is>
-      </c>
-      <c r="EF1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 4.id</t>
-        </is>
-      </c>
-      <c r="EG1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 4.type</t>
-        </is>
-      </c>
-      <c r="EH1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 4.select.id</t>
-        </is>
-      </c>
-      <c r="EI1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 4.select.name</t>
-        </is>
-      </c>
-      <c r="EJ1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 4.select.color</t>
-        </is>
-      </c>
-      <c r="EK1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Cơ sở.id</t>
-        </is>
-      </c>
-      <c r="EL1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Cơ sở.type</t>
-        </is>
-      </c>
-      <c r="EM1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Cơ sở.rollup.type</t>
-        </is>
-      </c>
-      <c r="EN1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Cơ sở.rollup.array</t>
-        </is>
-      </c>
-      <c r="EO1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Cơ sở.rollup.function</t>
-        </is>
-      </c>
-      <c r="EP1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 14.id</t>
-        </is>
-      </c>
-      <c r="EQ1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 14.type</t>
-        </is>
-      </c>
-      <c r="ER1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 14.select.id</t>
-        </is>
-      </c>
-      <c r="ES1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 14.select.name</t>
-        </is>
-      </c>
-      <c r="ET1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 14.select.color</t>
-        </is>
-      </c>
-      <c r="EU1" s="1" t="inlineStr">
-        <is>
-          <t>properties.STT.id</t>
-        </is>
-      </c>
-      <c r="EV1" s="1" t="inlineStr">
-        <is>
-          <t>properties.STT.type</t>
-        </is>
-      </c>
-      <c r="EW1" s="1" t="inlineStr">
-        <is>
-          <t>properties.STT.title</t>
-        </is>
-      </c>
-      <c r="EX1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 6.select</t>
-        </is>
-      </c>
-      <c r="EY1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 5.select</t>
-        </is>
-      </c>
-      <c r="EZ1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 11.select</t>
-        </is>
-      </c>
-      <c r="FA1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 3.select</t>
-        </is>
-      </c>
-      <c r="FB1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 12.select</t>
-        </is>
-      </c>
-      <c r="FC1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 10.select</t>
-        </is>
-      </c>
-      <c r="FD1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 2.select</t>
-        </is>
-      </c>
-      <c r="FE1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 7.select</t>
-        </is>
-      </c>
-      <c r="FF1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 1.select</t>
-        </is>
-      </c>
-      <c r="FG1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 9.select</t>
-        </is>
-      </c>
-      <c r="FH1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 16.select</t>
-        </is>
-      </c>
-      <c r="FI1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 15.select</t>
-        </is>
-      </c>
-      <c r="FJ1" s="1" t="inlineStr">
-        <is>
-          <t>properties.Ngày 13.select</t>
-        </is>
-      </c>
-      <c r="FK1" s="1" t="inlineStr">
+      <c r="FN1" s="1" t="inlineStr">
         <is>
           <t>properties.Ngày 8.select</t>
         </is>
       </c>
-      <c r="FL1" s="1" t="inlineStr">
+      <c r="FO1" s="1" t="inlineStr">
         <is>
           <t>properties.Ngày 4.select</t>
         </is>
       </c>
-      <c r="FM1" s="1" t="inlineStr">
+      <c r="FP1" s="1" t="inlineStr">
         <is>
           <t>properties.Ngày 14.select</t>
         </is>
@@ -1298,7 +1313,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-16T10:36:00.000Z</t>
+          <t>2024-07-17T16:52:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1852,124 +1867,136 @@
           <t>select</t>
         </is>
       </c>
-      <c r="DZ2" t="inlineStr"/>
+      <c r="DZ2" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
       <c r="EA2" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EB2" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EC2" t="inlineStr">
+        <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB2" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC2" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ED2" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EE2" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EF2" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EG2" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EH2" t="inlineStr">
+        <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG2" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH2" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="EI2" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EJ2" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EK2" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL2" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EM2" t="inlineStr">
+        <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL2" t="inlineStr">
+      <c r="EN2" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM2" t="inlineStr">
+      <c r="EO2" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN2" t="inlineStr">
+      <c r="EP2" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
-      <c r="EO2" t="inlineStr">
+      <c r="EQ2" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP2" t="inlineStr">
+      <c r="ER2" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ2" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER2" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ES2" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="ET2" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EU2" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EV2" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EW2" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV2" t="inlineStr">
+      <c r="EX2" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW2" t="inlineStr">
+      <c r="EY2" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX2" t="inlineStr"/>
-      <c r="EY2" t="inlineStr"/>
       <c r="EZ2" t="inlineStr"/>
       <c r="FA2" t="inlineStr"/>
       <c r="FB2" t="inlineStr"/>
@@ -1984,6 +2011,9 @@
       <c r="FK2" t="inlineStr"/>
       <c r="FL2" t="inlineStr"/>
       <c r="FM2" t="inlineStr"/>
+      <c r="FN2" t="inlineStr"/>
+      <c r="FO2" t="inlineStr"/>
+      <c r="FP2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2003,7 +2033,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-16T10:36:00.000Z</t>
+          <t>2024-07-17T16:52:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -2557,124 +2587,136 @@
           <t>select</t>
         </is>
       </c>
-      <c r="DZ3" t="inlineStr"/>
+      <c r="DZ3" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
       <c r="EA3" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EB3" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EC3" t="inlineStr">
+        <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB3" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC3" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ED3" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EE3" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EF3" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EG3" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EH3" t="inlineStr">
+        <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG3" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH3" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="EI3" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EJ3" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EK3" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL3" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EM3" t="inlineStr">
+        <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL3" t="inlineStr">
+      <c r="EN3" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM3" t="inlineStr">
+      <c r="EO3" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN3" t="inlineStr">
+      <c r="EP3" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
-      <c r="EO3" t="inlineStr">
+      <c r="EQ3" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP3" t="inlineStr">
+      <c r="ER3" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ3" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER3" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ES3" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="ET3" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EU3" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EV3" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EW3" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV3" t="inlineStr">
+      <c r="EX3" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW3" t="inlineStr">
+      <c r="EY3" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX3" t="inlineStr"/>
-      <c r="EY3" t="inlineStr"/>
       <c r="EZ3" t="inlineStr"/>
       <c r="FA3" t="inlineStr"/>
       <c r="FB3" t="inlineStr"/>
@@ -2689,6 +2731,9 @@
       <c r="FK3" t="inlineStr"/>
       <c r="FL3" t="inlineStr"/>
       <c r="FM3" t="inlineStr"/>
+      <c r="FN3" t="inlineStr"/>
+      <c r="FO3" t="inlineStr"/>
+      <c r="FP3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2708,7 +2753,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-16T10:36:00.000Z</t>
+          <t>2024-07-17T16:52:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -3262,124 +3307,136 @@
           <t>select</t>
         </is>
       </c>
-      <c r="DZ4" t="inlineStr"/>
+      <c r="DZ4" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
       <c r="EA4" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EB4" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EC4" t="inlineStr">
+        <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB4" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC4" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ED4" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EE4" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EF4" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EG4" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EH4" t="inlineStr">
+        <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG4" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH4" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="EI4" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EJ4" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EK4" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL4" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EM4" t="inlineStr">
+        <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL4" t="inlineStr">
+      <c r="EN4" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM4" t="inlineStr">
+      <c r="EO4" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN4" t="inlineStr">
+      <c r="EP4" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
-      <c r="EO4" t="inlineStr">
+      <c r="EQ4" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP4" t="inlineStr">
+      <c r="ER4" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ4" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER4" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ES4" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="ET4" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EU4" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EV4" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EW4" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV4" t="inlineStr">
+      <c r="EX4" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW4" t="inlineStr">
+      <c r="EY4" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX4" t="inlineStr"/>
-      <c r="EY4" t="inlineStr"/>
       <c r="EZ4" t="inlineStr"/>
       <c r="FA4" t="inlineStr"/>
       <c r="FB4" t="inlineStr"/>
@@ -3394,6 +3451,9 @@
       <c r="FK4" t="inlineStr"/>
       <c r="FL4" t="inlineStr"/>
       <c r="FM4" t="inlineStr"/>
+      <c r="FN4" t="inlineStr"/>
+      <c r="FO4" t="inlineStr"/>
+      <c r="FP4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3413,7 +3473,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-16T10:37:00.000Z</t>
+          <t>2024-07-17T16:52:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -3967,124 +4027,136 @@
           <t>select</t>
         </is>
       </c>
-      <c r="DZ5" t="inlineStr"/>
+      <c r="DZ5" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
       <c r="EA5" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EB5" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EC5" t="inlineStr">
+        <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB5" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC5" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ED5" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EE5" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EF5" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EG5" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EH5" t="inlineStr">
+        <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG5" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH5" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="EI5" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EJ5" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EK5" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL5" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EM5" t="inlineStr">
+        <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL5" t="inlineStr">
+      <c r="EN5" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM5" t="inlineStr">
+      <c r="EO5" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN5" t="inlineStr">
+      <c r="EP5" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
-      <c r="EO5" t="inlineStr">
+      <c r="EQ5" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP5" t="inlineStr">
+      <c r="ER5" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ5" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER5" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ES5" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="ET5" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EU5" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EV5" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EW5" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV5" t="inlineStr">
+      <c r="EX5" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW5" t="inlineStr">
+      <c r="EY5" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX5" t="inlineStr"/>
-      <c r="EY5" t="inlineStr"/>
       <c r="EZ5" t="inlineStr"/>
       <c r="FA5" t="inlineStr"/>
       <c r="FB5" t="inlineStr"/>
@@ -4099,6 +4171,9 @@
       <c r="FK5" t="inlineStr"/>
       <c r="FL5" t="inlineStr"/>
       <c r="FM5" t="inlineStr"/>
+      <c r="FN5" t="inlineStr"/>
+      <c r="FO5" t="inlineStr"/>
+      <c r="FP5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4517,87 +4592,87 @@
         </is>
       </c>
       <c r="DZ6" t="inlineStr"/>
-      <c r="EA6" t="inlineStr">
+      <c r="EA6" t="inlineStr"/>
+      <c r="EB6" t="inlineStr"/>
+      <c r="EC6" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB6" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC6" t="inlineStr"/>
-      <c r="ED6" t="inlineStr"/>
+      <c r="ED6" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE6" t="inlineStr"/>
-      <c r="EF6" t="inlineStr">
+      <c r="EF6" t="inlineStr"/>
+      <c r="EG6" t="inlineStr"/>
+      <c r="EH6" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG6" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH6" t="inlineStr"/>
-      <c r="EI6" t="inlineStr"/>
+      <c r="EI6" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ6" t="inlineStr"/>
-      <c r="EK6" t="inlineStr">
+      <c r="EK6" t="inlineStr"/>
+      <c r="EL6" t="inlineStr"/>
+      <c r="EM6" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL6" t="inlineStr">
+      <c r="EN6" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM6" t="inlineStr">
+      <c r="EO6" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN6" t="inlineStr">
+      <c r="EP6" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
-      <c r="EO6" t="inlineStr">
+      <c r="EQ6" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP6" t="inlineStr">
+      <c r="ER6" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ6" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER6" t="inlineStr"/>
-      <c r="ES6" t="inlineStr"/>
+      <c r="ES6" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET6" t="inlineStr"/>
-      <c r="EU6" t="inlineStr">
+      <c r="EU6" t="inlineStr"/>
+      <c r="EV6" t="inlineStr"/>
+      <c r="EW6" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV6" t="inlineStr">
+      <c r="EX6" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW6" t="inlineStr">
+      <c r="EY6" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX6" t="inlineStr"/>
-      <c r="EY6" t="inlineStr"/>
       <c r="EZ6" t="inlineStr"/>
       <c r="FA6" t="inlineStr"/>
       <c r="FB6" t="inlineStr"/>
@@ -4612,6 +4687,9 @@
       <c r="FK6" t="inlineStr"/>
       <c r="FL6" t="inlineStr"/>
       <c r="FM6" t="inlineStr"/>
+      <c r="FN6" t="inlineStr"/>
+      <c r="FO6" t="inlineStr"/>
+      <c r="FP6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5030,87 +5108,87 @@
         </is>
       </c>
       <c r="DZ7" t="inlineStr"/>
-      <c r="EA7" t="inlineStr">
+      <c r="EA7" t="inlineStr"/>
+      <c r="EB7" t="inlineStr"/>
+      <c r="EC7" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB7" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC7" t="inlineStr"/>
-      <c r="ED7" t="inlineStr"/>
+      <c r="ED7" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE7" t="inlineStr"/>
-      <c r="EF7" t="inlineStr">
+      <c r="EF7" t="inlineStr"/>
+      <c r="EG7" t="inlineStr"/>
+      <c r="EH7" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG7" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH7" t="inlineStr"/>
-      <c r="EI7" t="inlineStr"/>
+      <c r="EI7" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ7" t="inlineStr"/>
-      <c r="EK7" t="inlineStr">
+      <c r="EK7" t="inlineStr"/>
+      <c r="EL7" t="inlineStr"/>
+      <c r="EM7" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL7" t="inlineStr">
+      <c r="EN7" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM7" t="inlineStr">
+      <c r="EO7" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN7" t="inlineStr">
+      <c r="EP7" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
-      <c r="EO7" t="inlineStr">
+      <c r="EQ7" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP7" t="inlineStr">
+      <c r="ER7" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ7" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER7" t="inlineStr"/>
-      <c r="ES7" t="inlineStr"/>
+      <c r="ES7" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET7" t="inlineStr"/>
-      <c r="EU7" t="inlineStr">
+      <c r="EU7" t="inlineStr"/>
+      <c r="EV7" t="inlineStr"/>
+      <c r="EW7" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV7" t="inlineStr">
+      <c r="EX7" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW7" t="inlineStr">
+      <c r="EY7" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX7" t="inlineStr"/>
-      <c r="EY7" t="inlineStr"/>
       <c r="EZ7" t="inlineStr"/>
       <c r="FA7" t="inlineStr"/>
       <c r="FB7" t="inlineStr"/>
@@ -5125,6 +5203,9 @@
       <c r="FK7" t="inlineStr"/>
       <c r="FL7" t="inlineStr"/>
       <c r="FM7" t="inlineStr"/>
+      <c r="FN7" t="inlineStr"/>
+      <c r="FO7" t="inlineStr"/>
+      <c r="FP7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5543,87 +5624,87 @@
         </is>
       </c>
       <c r="DZ8" t="inlineStr"/>
-      <c r="EA8" t="inlineStr">
+      <c r="EA8" t="inlineStr"/>
+      <c r="EB8" t="inlineStr"/>
+      <c r="EC8" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB8" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC8" t="inlineStr"/>
-      <c r="ED8" t="inlineStr"/>
+      <c r="ED8" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE8" t="inlineStr"/>
-      <c r="EF8" t="inlineStr">
+      <c r="EF8" t="inlineStr"/>
+      <c r="EG8" t="inlineStr"/>
+      <c r="EH8" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG8" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH8" t="inlineStr"/>
-      <c r="EI8" t="inlineStr"/>
+      <c r="EI8" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ8" t="inlineStr"/>
-      <c r="EK8" t="inlineStr">
+      <c r="EK8" t="inlineStr"/>
+      <c r="EL8" t="inlineStr"/>
+      <c r="EM8" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL8" t="inlineStr">
+      <c r="EN8" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM8" t="inlineStr">
+      <c r="EO8" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN8" t="inlineStr">
+      <c r="EP8" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
         </is>
       </c>
-      <c r="EO8" t="inlineStr">
+      <c r="EQ8" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP8" t="inlineStr">
+      <c r="ER8" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ8" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER8" t="inlineStr"/>
-      <c r="ES8" t="inlineStr"/>
+      <c r="ES8" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET8" t="inlineStr"/>
-      <c r="EU8" t="inlineStr">
+      <c r="EU8" t="inlineStr"/>
+      <c r="EV8" t="inlineStr"/>
+      <c r="EW8" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV8" t="inlineStr">
+      <c r="EX8" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW8" t="inlineStr">
+      <c r="EY8" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX8" t="inlineStr"/>
-      <c r="EY8" t="inlineStr"/>
       <c r="EZ8" t="inlineStr"/>
       <c r="FA8" t="inlineStr"/>
       <c r="FB8" t="inlineStr"/>
@@ -5638,6 +5719,9 @@
       <c r="FK8" t="inlineStr"/>
       <c r="FL8" t="inlineStr"/>
       <c r="FM8" t="inlineStr"/>
+      <c r="FN8" t="inlineStr"/>
+      <c r="FO8" t="inlineStr"/>
+      <c r="FP8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -6056,87 +6140,87 @@
         </is>
       </c>
       <c r="DZ9" t="inlineStr"/>
-      <c r="EA9" t="inlineStr">
+      <c r="EA9" t="inlineStr"/>
+      <c r="EB9" t="inlineStr"/>
+      <c r="EC9" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB9" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC9" t="inlineStr"/>
-      <c r="ED9" t="inlineStr"/>
+      <c r="ED9" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE9" t="inlineStr"/>
-      <c r="EF9" t="inlineStr">
+      <c r="EF9" t="inlineStr"/>
+      <c r="EG9" t="inlineStr"/>
+      <c r="EH9" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG9" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH9" t="inlineStr"/>
-      <c r="EI9" t="inlineStr"/>
+      <c r="EI9" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ9" t="inlineStr"/>
-      <c r="EK9" t="inlineStr">
+      <c r="EK9" t="inlineStr"/>
+      <c r="EL9" t="inlineStr"/>
+      <c r="EM9" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL9" t="inlineStr">
+      <c r="EN9" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM9" t="inlineStr">
+      <c r="EO9" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN9" t="inlineStr">
+      <c r="EP9" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
         </is>
       </c>
-      <c r="EO9" t="inlineStr">
+      <c r="EQ9" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP9" t="inlineStr">
+      <c r="ER9" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ9" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER9" t="inlineStr"/>
-      <c r="ES9" t="inlineStr"/>
+      <c r="ES9" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET9" t="inlineStr"/>
-      <c r="EU9" t="inlineStr">
+      <c r="EU9" t="inlineStr"/>
+      <c r="EV9" t="inlineStr"/>
+      <c r="EW9" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV9" t="inlineStr">
+      <c r="EX9" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW9" t="inlineStr">
+      <c r="EY9" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX9" t="inlineStr"/>
-      <c r="EY9" t="inlineStr"/>
       <c r="EZ9" t="inlineStr"/>
       <c r="FA9" t="inlineStr"/>
       <c r="FB9" t="inlineStr"/>
@@ -6151,6 +6235,9 @@
       <c r="FK9" t="inlineStr"/>
       <c r="FL9" t="inlineStr"/>
       <c r="FM9" t="inlineStr"/>
+      <c r="FN9" t="inlineStr"/>
+      <c r="FO9" t="inlineStr"/>
+      <c r="FP9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -6581,87 +6668,87 @@
         </is>
       </c>
       <c r="DZ10" t="inlineStr"/>
-      <c r="EA10" t="inlineStr">
+      <c r="EA10" t="inlineStr"/>
+      <c r="EB10" t="inlineStr"/>
+      <c r="EC10" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB10" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC10" t="inlineStr"/>
-      <c r="ED10" t="inlineStr"/>
+      <c r="ED10" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE10" t="inlineStr"/>
-      <c r="EF10" t="inlineStr">
+      <c r="EF10" t="inlineStr"/>
+      <c r="EG10" t="inlineStr"/>
+      <c r="EH10" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG10" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH10" t="inlineStr"/>
-      <c r="EI10" t="inlineStr"/>
+      <c r="EI10" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ10" t="inlineStr"/>
-      <c r="EK10" t="inlineStr">
+      <c r="EK10" t="inlineStr"/>
+      <c r="EL10" t="inlineStr"/>
+      <c r="EM10" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL10" t="inlineStr">
+      <c r="EN10" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM10" t="inlineStr">
+      <c r="EO10" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN10" t="inlineStr">
+      <c r="EP10" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
-      <c r="EO10" t="inlineStr">
+      <c r="EQ10" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP10" t="inlineStr">
+      <c r="ER10" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ10" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER10" t="inlineStr"/>
-      <c r="ES10" t="inlineStr"/>
+      <c r="ES10" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET10" t="inlineStr"/>
-      <c r="EU10" t="inlineStr">
+      <c r="EU10" t="inlineStr"/>
+      <c r="EV10" t="inlineStr"/>
+      <c r="EW10" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV10" t="inlineStr">
+      <c r="EX10" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW10" t="inlineStr">
+      <c r="EY10" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX10" t="inlineStr"/>
-      <c r="EY10" t="inlineStr"/>
       <c r="EZ10" t="inlineStr"/>
       <c r="FA10" t="inlineStr"/>
       <c r="FB10" t="inlineStr"/>
@@ -6676,6 +6763,9 @@
       <c r="FK10" t="inlineStr"/>
       <c r="FL10" t="inlineStr"/>
       <c r="FM10" t="inlineStr"/>
+      <c r="FN10" t="inlineStr"/>
+      <c r="FO10" t="inlineStr"/>
+      <c r="FP10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -7094,87 +7184,87 @@
         </is>
       </c>
       <c r="DZ11" t="inlineStr"/>
-      <c r="EA11" t="inlineStr">
+      <c r="EA11" t="inlineStr"/>
+      <c r="EB11" t="inlineStr"/>
+      <c r="EC11" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB11" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC11" t="inlineStr"/>
-      <c r="ED11" t="inlineStr"/>
+      <c r="ED11" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE11" t="inlineStr"/>
-      <c r="EF11" t="inlineStr">
+      <c r="EF11" t="inlineStr"/>
+      <c r="EG11" t="inlineStr"/>
+      <c r="EH11" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG11" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH11" t="inlineStr"/>
-      <c r="EI11" t="inlineStr"/>
+      <c r="EI11" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ11" t="inlineStr"/>
-      <c r="EK11" t="inlineStr">
+      <c r="EK11" t="inlineStr"/>
+      <c r="EL11" t="inlineStr"/>
+      <c r="EM11" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL11" t="inlineStr">
+      <c r="EN11" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM11" t="inlineStr">
+      <c r="EO11" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN11" t="inlineStr">
+      <c r="EP11" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
-      <c r="EO11" t="inlineStr">
+      <c r="EQ11" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP11" t="inlineStr">
+      <c r="ER11" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ11" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER11" t="inlineStr"/>
-      <c r="ES11" t="inlineStr"/>
+      <c r="ES11" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET11" t="inlineStr"/>
-      <c r="EU11" t="inlineStr">
+      <c r="EU11" t="inlineStr"/>
+      <c r="EV11" t="inlineStr"/>
+      <c r="EW11" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV11" t="inlineStr">
+      <c r="EX11" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW11" t="inlineStr">
+      <c r="EY11" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX11" t="inlineStr"/>
-      <c r="EY11" t="inlineStr"/>
       <c r="EZ11" t="inlineStr"/>
       <c r="FA11" t="inlineStr"/>
       <c r="FB11" t="inlineStr"/>
@@ -7189,6 +7279,9 @@
       <c r="FK11" t="inlineStr"/>
       <c r="FL11" t="inlineStr"/>
       <c r="FM11" t="inlineStr"/>
+      <c r="FN11" t="inlineStr"/>
+      <c r="FO11" t="inlineStr"/>
+      <c r="FP11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -7208,7 +7301,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-16T10:36:00.000Z</t>
+          <t>2024-07-17T16:52:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -7762,124 +7855,136 @@
           <t>select</t>
         </is>
       </c>
-      <c r="DZ12" t="inlineStr"/>
+      <c r="DZ12" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
       <c r="EA12" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EB12" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EC12" t="inlineStr">
+        <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB12" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC12" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ED12" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EE12" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EF12" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EG12" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EH12" t="inlineStr">
+        <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG12" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH12" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="EI12" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EJ12" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EK12" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL12" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EM12" t="inlineStr">
+        <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL12" t="inlineStr">
+      <c r="EN12" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM12" t="inlineStr">
+      <c r="EO12" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN12" t="inlineStr">
+      <c r="EP12" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
-      <c r="EO12" t="inlineStr">
+      <c r="EQ12" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP12" t="inlineStr">
+      <c r="ER12" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ12" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER12" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ES12" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="ET12" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EU12" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EV12" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EW12" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV12" t="inlineStr">
+      <c r="EX12" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW12" t="inlineStr">
+      <c r="EY12" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX12" t="inlineStr"/>
-      <c r="EY12" t="inlineStr"/>
       <c r="EZ12" t="inlineStr"/>
       <c r="FA12" t="inlineStr"/>
       <c r="FB12" t="inlineStr"/>
@@ -7894,6 +7999,9 @@
       <c r="FK12" t="inlineStr"/>
       <c r="FL12" t="inlineStr"/>
       <c r="FM12" t="inlineStr"/>
+      <c r="FN12" t="inlineStr"/>
+      <c r="FO12" t="inlineStr"/>
+      <c r="FP12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -7913,7 +8021,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-16T10:37:00.000Z</t>
+          <t>2024-07-17T16:52:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -8467,124 +8575,136 @@
           <t>select</t>
         </is>
       </c>
-      <c r="DZ13" t="inlineStr"/>
+      <c r="DZ13" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
       <c r="EA13" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EB13" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EC13" t="inlineStr">
+        <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB13" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC13" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ED13" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EE13" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EF13" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EG13" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EH13" t="inlineStr">
+        <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG13" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH13" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="EI13" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EJ13" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EK13" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL13" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EM13" t="inlineStr">
+        <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL13" t="inlineStr">
+      <c r="EN13" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM13" t="inlineStr">
+      <c r="EO13" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN13" t="inlineStr">
+      <c r="EP13" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
-      <c r="EO13" t="inlineStr">
+      <c r="EQ13" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP13" t="inlineStr">
+      <c r="ER13" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ13" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER13" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ES13" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="ET13" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EU13" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EV13" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EW13" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV13" t="inlineStr">
+      <c r="EX13" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW13" t="inlineStr">
+      <c r="EY13" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX13" t="inlineStr"/>
-      <c r="EY13" t="inlineStr"/>
       <c r="EZ13" t="inlineStr"/>
       <c r="FA13" t="inlineStr"/>
       <c r="FB13" t="inlineStr"/>
@@ -8599,6 +8719,9 @@
       <c r="FK13" t="inlineStr"/>
       <c r="FL13" t="inlineStr"/>
       <c r="FM13" t="inlineStr"/>
+      <c r="FN13" t="inlineStr"/>
+      <c r="FO13" t="inlineStr"/>
+      <c r="FP13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -9017,87 +9140,87 @@
         </is>
       </c>
       <c r="DZ14" t="inlineStr"/>
-      <c r="EA14" t="inlineStr">
+      <c r="EA14" t="inlineStr"/>
+      <c r="EB14" t="inlineStr"/>
+      <c r="EC14" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB14" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC14" t="inlineStr"/>
-      <c r="ED14" t="inlineStr"/>
+      <c r="ED14" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE14" t="inlineStr"/>
-      <c r="EF14" t="inlineStr">
+      <c r="EF14" t="inlineStr"/>
+      <c r="EG14" t="inlineStr"/>
+      <c r="EH14" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG14" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH14" t="inlineStr"/>
-      <c r="EI14" t="inlineStr"/>
+      <c r="EI14" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ14" t="inlineStr"/>
-      <c r="EK14" t="inlineStr">
+      <c r="EK14" t="inlineStr"/>
+      <c r="EL14" t="inlineStr"/>
+      <c r="EM14" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL14" t="inlineStr">
+      <c r="EN14" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM14" t="inlineStr">
+      <c r="EO14" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN14" t="inlineStr">
+      <c r="EP14" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
         </is>
       </c>
-      <c r="EO14" t="inlineStr">
+      <c r="EQ14" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP14" t="inlineStr">
+      <c r="ER14" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ14" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER14" t="inlineStr"/>
-      <c r="ES14" t="inlineStr"/>
+      <c r="ES14" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET14" t="inlineStr"/>
-      <c r="EU14" t="inlineStr">
+      <c r="EU14" t="inlineStr"/>
+      <c r="EV14" t="inlineStr"/>
+      <c r="EW14" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV14" t="inlineStr">
+      <c r="EX14" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW14" t="inlineStr">
+      <c r="EY14" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX14" t="inlineStr"/>
-      <c r="EY14" t="inlineStr"/>
       <c r="EZ14" t="inlineStr"/>
       <c r="FA14" t="inlineStr"/>
       <c r="FB14" t="inlineStr"/>
@@ -9112,6 +9235,9 @@
       <c r="FK14" t="inlineStr"/>
       <c r="FL14" t="inlineStr"/>
       <c r="FM14" t="inlineStr"/>
+      <c r="FN14" t="inlineStr"/>
+      <c r="FO14" t="inlineStr"/>
+      <c r="FP14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -9131,7 +9257,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-16T10:37:00.000Z</t>
+          <t>2024-07-17T16:52:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -9685,124 +9811,136 @@
           <t>select</t>
         </is>
       </c>
-      <c r="DZ15" t="inlineStr"/>
+      <c r="DZ15" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
       <c r="EA15" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EB15" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EC15" t="inlineStr">
+        <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB15" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC15" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ED15" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EE15" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EF15" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EG15" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EH15" t="inlineStr">
+        <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG15" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH15" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="EI15" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EJ15" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EK15" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL15" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EM15" t="inlineStr">
+        <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL15" t="inlineStr">
+      <c r="EN15" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM15" t="inlineStr">
+      <c r="EO15" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN15" t="inlineStr">
+      <c r="EP15" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
-      <c r="EO15" t="inlineStr">
+      <c r="EQ15" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP15" t="inlineStr">
+      <c r="ER15" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ15" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER15" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ES15" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="ET15" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EU15" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EV15" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EW15" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV15" t="inlineStr">
+      <c r="EX15" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW15" t="inlineStr">
+      <c r="EY15" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX15" t="inlineStr"/>
-      <c r="EY15" t="inlineStr"/>
       <c r="EZ15" t="inlineStr"/>
       <c r="FA15" t="inlineStr"/>
       <c r="FB15" t="inlineStr"/>
@@ -9817,6 +9955,9 @@
       <c r="FK15" t="inlineStr"/>
       <c r="FL15" t="inlineStr"/>
       <c r="FM15" t="inlineStr"/>
+      <c r="FN15" t="inlineStr"/>
+      <c r="FO15" t="inlineStr"/>
+      <c r="FP15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -9836,7 +9977,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-16T10:36:00.000Z</t>
+          <t>2024-07-17T16:52:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -10390,124 +10531,136 @@
           <t>select</t>
         </is>
       </c>
-      <c r="DZ16" t="inlineStr"/>
+      <c r="DZ16" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
       <c r="EA16" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EB16" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EC16" t="inlineStr">
+        <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB16" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC16" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ED16" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EE16" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EF16" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EG16" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EH16" t="inlineStr">
+        <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG16" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH16" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="EI16" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EJ16" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EK16" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL16" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EM16" t="inlineStr">
+        <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL16" t="inlineStr">
+      <c r="EN16" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM16" t="inlineStr">
+      <c r="EO16" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN16" t="inlineStr">
+      <c r="EP16" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
-      <c r="EO16" t="inlineStr">
+      <c r="EQ16" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP16" t="inlineStr">
+      <c r="ER16" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ16" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER16" t="inlineStr">
+      <c r="ES16" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
+      <c r="ET16" t="inlineStr">
         <is>
           <t>VRLp</t>
         </is>
       </c>
-      <c r="ES16" t="inlineStr">
+      <c r="EU16" t="inlineStr">
         <is>
           <t>Nghỉ có phép</t>
         </is>
       </c>
-      <c r="ET16" t="inlineStr">
+      <c r="EV16" t="inlineStr">
         <is>
           <t>blue</t>
         </is>
       </c>
-      <c r="EU16" t="inlineStr">
+      <c r="EW16" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV16" t="inlineStr">
+      <c r="EX16" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW16" t="inlineStr">
+      <c r="EY16" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX16" t="inlineStr"/>
-      <c r="EY16" t="inlineStr"/>
       <c r="EZ16" t="inlineStr"/>
       <c r="FA16" t="inlineStr"/>
       <c r="FB16" t="inlineStr"/>
@@ -10522,6 +10675,9 @@
       <c r="FK16" t="inlineStr"/>
       <c r="FL16" t="inlineStr"/>
       <c r="FM16" t="inlineStr"/>
+      <c r="FN16" t="inlineStr"/>
+      <c r="FO16" t="inlineStr"/>
+      <c r="FP16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -10940,87 +11096,87 @@
         </is>
       </c>
       <c r="DZ17" t="inlineStr"/>
-      <c r="EA17" t="inlineStr">
+      <c r="EA17" t="inlineStr"/>
+      <c r="EB17" t="inlineStr"/>
+      <c r="EC17" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB17" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC17" t="inlineStr"/>
-      <c r="ED17" t="inlineStr"/>
+      <c r="ED17" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE17" t="inlineStr"/>
-      <c r="EF17" t="inlineStr">
+      <c r="EF17" t="inlineStr"/>
+      <c r="EG17" t="inlineStr"/>
+      <c r="EH17" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG17" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH17" t="inlineStr"/>
-      <c r="EI17" t="inlineStr"/>
+      <c r="EI17" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ17" t="inlineStr"/>
-      <c r="EK17" t="inlineStr">
+      <c r="EK17" t="inlineStr"/>
+      <c r="EL17" t="inlineStr"/>
+      <c r="EM17" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL17" t="inlineStr">
+      <c r="EN17" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM17" t="inlineStr">
+      <c r="EO17" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN17" t="inlineStr">
+      <c r="EP17" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
-      <c r="EO17" t="inlineStr">
+      <c r="EQ17" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP17" t="inlineStr">
+      <c r="ER17" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ17" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER17" t="inlineStr"/>
-      <c r="ES17" t="inlineStr"/>
+      <c r="ES17" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET17" t="inlineStr"/>
-      <c r="EU17" t="inlineStr">
+      <c r="EU17" t="inlineStr"/>
+      <c r="EV17" t="inlineStr"/>
+      <c r="EW17" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV17" t="inlineStr">
+      <c r="EX17" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW17" t="inlineStr">
+      <c r="EY17" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX17" t="inlineStr"/>
-      <c r="EY17" t="inlineStr"/>
       <c r="EZ17" t="inlineStr"/>
       <c r="FA17" t="inlineStr"/>
       <c r="FB17" t="inlineStr"/>
@@ -11035,6 +11191,9 @@
       <c r="FK17" t="inlineStr"/>
       <c r="FL17" t="inlineStr"/>
       <c r="FM17" t="inlineStr"/>
+      <c r="FN17" t="inlineStr"/>
+      <c r="FO17" t="inlineStr"/>
+      <c r="FP17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -11453,87 +11612,87 @@
         </is>
       </c>
       <c r="DZ18" t="inlineStr"/>
-      <c r="EA18" t="inlineStr">
+      <c r="EA18" t="inlineStr"/>
+      <c r="EB18" t="inlineStr"/>
+      <c r="EC18" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB18" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC18" t="inlineStr"/>
-      <c r="ED18" t="inlineStr"/>
+      <c r="ED18" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE18" t="inlineStr"/>
-      <c r="EF18" t="inlineStr">
+      <c r="EF18" t="inlineStr"/>
+      <c r="EG18" t="inlineStr"/>
+      <c r="EH18" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG18" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH18" t="inlineStr"/>
-      <c r="EI18" t="inlineStr"/>
+      <c r="EI18" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ18" t="inlineStr"/>
-      <c r="EK18" t="inlineStr">
+      <c r="EK18" t="inlineStr"/>
+      <c r="EL18" t="inlineStr"/>
+      <c r="EM18" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL18" t="inlineStr">
+      <c r="EN18" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM18" t="inlineStr">
+      <c r="EO18" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN18" t="inlineStr">
+      <c r="EP18" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
         </is>
       </c>
-      <c r="EO18" t="inlineStr">
+      <c r="EQ18" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP18" t="inlineStr">
+      <c r="ER18" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ18" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER18" t="inlineStr"/>
-      <c r="ES18" t="inlineStr"/>
+      <c r="ES18" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET18" t="inlineStr"/>
-      <c r="EU18" t="inlineStr">
+      <c r="EU18" t="inlineStr"/>
+      <c r="EV18" t="inlineStr"/>
+      <c r="EW18" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV18" t="inlineStr">
+      <c r="EX18" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW18" t="inlineStr">
+      <c r="EY18" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX18" t="inlineStr"/>
-      <c r="EY18" t="inlineStr"/>
       <c r="EZ18" t="inlineStr"/>
       <c r="FA18" t="inlineStr"/>
       <c r="FB18" t="inlineStr"/>
@@ -11548,6 +11707,9 @@
       <c r="FK18" t="inlineStr"/>
       <c r="FL18" t="inlineStr"/>
       <c r="FM18" t="inlineStr"/>
+      <c r="FN18" t="inlineStr"/>
+      <c r="FO18" t="inlineStr"/>
+      <c r="FP18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -11966,87 +12128,87 @@
         </is>
       </c>
       <c r="DZ19" t="inlineStr"/>
-      <c r="EA19" t="inlineStr">
+      <c r="EA19" t="inlineStr"/>
+      <c r="EB19" t="inlineStr"/>
+      <c r="EC19" t="inlineStr">
         <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB19" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC19" t="inlineStr"/>
-      <c r="ED19" t="inlineStr"/>
+      <c r="ED19" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EE19" t="inlineStr"/>
-      <c r="EF19" t="inlineStr">
+      <c r="EF19" t="inlineStr"/>
+      <c r="EG19" t="inlineStr"/>
+      <c r="EH19" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG19" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH19" t="inlineStr"/>
-      <c r="EI19" t="inlineStr"/>
+      <c r="EI19" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="EJ19" t="inlineStr"/>
-      <c r="EK19" t="inlineStr">
+      <c r="EK19" t="inlineStr"/>
+      <c r="EL19" t="inlineStr"/>
+      <c r="EM19" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL19" t="inlineStr">
+      <c r="EN19" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM19" t="inlineStr">
+      <c r="EO19" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN19" t="inlineStr">
+      <c r="EP19" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
         </is>
       </c>
-      <c r="EO19" t="inlineStr">
+      <c r="EQ19" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP19" t="inlineStr">
+      <c r="ER19" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ19" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER19" t="inlineStr"/>
-      <c r="ES19" t="inlineStr"/>
+      <c r="ES19" t="inlineStr">
+        <is>
+          <t>select</t>
+        </is>
+      </c>
       <c r="ET19" t="inlineStr"/>
-      <c r="EU19" t="inlineStr">
+      <c r="EU19" t="inlineStr"/>
+      <c r="EV19" t="inlineStr"/>
+      <c r="EW19" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV19" t="inlineStr">
+      <c r="EX19" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW19" t="inlineStr">
+      <c r="EY19" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX19" t="inlineStr"/>
-      <c r="EY19" t="inlineStr"/>
       <c r="EZ19" t="inlineStr"/>
       <c r="FA19" t="inlineStr"/>
       <c r="FB19" t="inlineStr"/>
@@ -12061,6 +12223,9 @@
       <c r="FK19" t="inlineStr"/>
       <c r="FL19" t="inlineStr"/>
       <c r="FM19" t="inlineStr"/>
+      <c r="FN19" t="inlineStr"/>
+      <c r="FO19" t="inlineStr"/>
+      <c r="FP19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -12080,7 +12245,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-16T10:37:00.000Z</t>
+          <t>2024-07-17T16:52:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -12634,124 +12799,136 @@
           <t>select</t>
         </is>
       </c>
-      <c r="DZ20" t="inlineStr"/>
+      <c r="DZ20" t="inlineStr">
+        <is>
+          <t>DjwF</t>
+        </is>
+      </c>
       <c r="EA20" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EB20" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EC20" t="inlineStr">
+        <is>
           <t>zBvN</t>
         </is>
       </c>
-      <c r="EB20" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EC20" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ED20" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EE20" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EF20" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EG20" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EH20" t="inlineStr">
+        <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="EG20" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="EH20" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="EI20" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="EJ20" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EK20" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EL20" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EM20" t="inlineStr">
+        <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="EL20" t="inlineStr">
+      <c r="EN20" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="EM20" t="inlineStr">
+      <c r="EO20" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="EN20" t="inlineStr">
+      <c r="EP20" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
-      <c r="EO20" t="inlineStr">
+      <c r="EQ20" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="EP20" t="inlineStr">
+      <c r="ER20" t="inlineStr">
         <is>
           <t>~q%3Ax</t>
         </is>
       </c>
-      <c r="EQ20" t="inlineStr">
-        <is>
-          <t>select</t>
-        </is>
-      </c>
-      <c r="ER20" t="inlineStr">
-        <is>
-          <t>DjwF</t>
-        </is>
-      </c>
       <c r="ES20" t="inlineStr">
         <is>
-          <t>Đầy đủ</t>
+          <t>select</t>
         </is>
       </c>
       <c r="ET20" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>DjwF</t>
         </is>
       </c>
       <c r="EU20" t="inlineStr">
         <is>
+          <t>Đầy đủ</t>
+        </is>
+      </c>
+      <c r="EV20" t="inlineStr">
+        <is>
+          <t>pink</t>
+        </is>
+      </c>
+      <c r="EW20" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EV20" t="inlineStr">
+      <c r="EX20" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="EW20" t="inlineStr">
+      <c r="EY20" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="EX20" t="inlineStr"/>
-      <c r="EY20" t="inlineStr"/>
       <c r="EZ20" t="inlineStr"/>
       <c r="FA20" t="inlineStr"/>
       <c r="FB20" t="inlineStr"/>
@@ -12766,6 +12943,9 @@
       <c r="FK20" t="inlineStr"/>
       <c r="FL20" t="inlineStr"/>
       <c r="FM20" t="inlineStr"/>
+      <c r="FN20" t="inlineStr"/>
+      <c r="FO20" t="inlineStr"/>
+      <c r="FP20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>